<commit_message>
colocando os valores de dominio
</commit_message>
<xml_diff>
--- a/docs/Guia_de_ids/Lista_de_Ids.xlsx
+++ b/docs/Guia_de_ids/Lista_de_Ids.xlsx
@@ -5,37 +5,28 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zirondi\Downloads\trabalho-integrado-2020-1-grupo-4\Imagens\Guia_de_ids\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ReservaGB\Desktop\psw\trabalho-integrado-2020-1-grupo-4\docs\Guia_de_ids\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2DB131-6768-4462-A754-8D6FF0E2D8E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47476B7E-0736-4CD3-8EED-6FC12F40F741}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{71A03D64-A901-4312-B88C-EC945196CD5F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{71A03D64-A901-4312-B88C-EC945196CD5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Telas" sheetId="3" r:id="rId1"/>
     <sheet name="Por Telas" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
   <si>
     <t>T01</t>
   </si>
@@ -371,13 +362,55 @@
   </si>
   <si>
     <t>Tabela de Templates de Formulários</t>
+  </si>
+  <si>
+    <t>Dominio</t>
+  </si>
+  <si>
+    <t>Válido</t>
+  </si>
+  <si>
+    <t>Inválido</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Form</t>
+  </si>
+  <si>
+    <t>50 char</t>
+  </si>
+  <si>
+    <t>3 char</t>
+  </si>
+  <si>
+    <t>Obrigatorio</t>
+  </si>
+  <si>
+    <t>Não obrigatorio</t>
+  </si>
+  <si>
+    <t>Expressão Regular : ^([a-zA-Z0-9_\-\.]+)@((\[[0-9]{1,3}\.[0-9]{1,3}\.[0-9]{1,3}\.)|(([a-zA-Z0-9\-]+\.)+))([a-zA-Z]{2,4}|[0-9]{1,3})$</t>
+  </si>
+  <si>
+    <t>Não contemplar as expressão regular</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Valor minimo</t>
+  </si>
+  <si>
+    <t>Valor máximo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,16 +424,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -408,13 +471,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,9 +835,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0614E616-5480-4700-8D6E-6AFC0B0ACF2C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -741,814 +845,1268 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D5DBAC-F946-4952-A064-CD386759A3EC}">
-  <dimension ref="A1:K56"/>
+  <dimension ref="B2:L57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32:G32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="46.5546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="58.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="51" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="108.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="2" spans="2:12">
+      <c r="B2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="F2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="2:12">
+      <c r="B4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="2:12">
+      <c r="B5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="2:12" ht="16.5" customHeight="1">
+      <c r="B6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="2:12">
+      <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="F7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="2:12" ht="16.5" customHeight="1">
+      <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="F8" s="4"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="F9" s="4"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="F10" s="4"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="2:12">
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E11" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="F11" s="4"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="2:12">
+      <c r="B12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C12" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="F12" s="4"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="2:12">
+      <c r="B13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E13" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="F13" s="4"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="2:12">
+      <c r="B14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E14" s="9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C15" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D15" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E15" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="F15" s="4"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E16" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="C17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E17" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="C18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E18" s="9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C19" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E19" s="9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="F19" s="4"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="C20" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E20" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="F20" s="4"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C21" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D21" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E21" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="F21" s="4"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C22" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E22" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="F22" s="4"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="C23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E23" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="F23" s="4"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E24" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="F24" s="4"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C25" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E25" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="F25" s="4"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E26" s="9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="F26" s="4"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="C27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E27" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="F27" s="4"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="B28" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="C28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E28" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="F28" s="4"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E29" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="F29" s="4"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="C30" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E30" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="F30" s="4"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="C31" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E31" s="9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="F31" s="4"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="B32" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C32" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D32" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E32" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="F32" s="4"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="C33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E33" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="F33" s="4"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B33" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="C34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E34" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="F34" s="4"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B34" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="C35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E35" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="F35" s="4"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B35" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="C36" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E36" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="F36" s="4"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B36" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="C37" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E37" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="F37" s="4"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="2:12">
+      <c r="B38" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C38" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E38" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="F38" s="4"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="4"/>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C39" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E39" s="9" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="F39" s="4"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="2:12">
+      <c r="B40" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="C40" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E40" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="F40" s="4"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="2:12">
+      <c r="B41" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B40" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C41" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E41" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="F41" s="4"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="2:12">
+      <c r="B42" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C42" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D42" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E42" s="9" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="F42" s="4"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="B43" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C43" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D43" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E43" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="F43" s="4"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="4"/>
+    </row>
+    <row r="44" spans="2:12">
+      <c r="B44" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C44" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D44" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E44" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="F44" s="4"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="B45" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="C45" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E45" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="F45" s="4"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="4"/>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="B46" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C46" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D46" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E46" s="9" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="F46" s="4"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="B47" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C47" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D47" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E47" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="F47" s="4"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="4"/>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="C48" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E48" s="9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="F48" s="4"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="2:12">
+      <c r="B49" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B48" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="C49" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E49" s="9" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="F49" s="4"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="2:12">
+      <c r="B50" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B49" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="C50" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E50" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="F50" s="4"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="B51" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B50" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="C51" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E51" s="9" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="F51" s="4"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="B52" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B51" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="C52" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E52" s="9" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="F52" s="4"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="2:12">
+      <c r="B53" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="B52" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="C53" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E53" s="9" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="F53" s="4"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="B54" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C54" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D54" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E54" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="F54" s="4"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="4"/>
+    </row>
+    <row r="55" spans="2:12">
+      <c r="B55" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="C55" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E55" s="9" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="F55" s="4"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="2:12">
+      <c r="B56" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B55" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="C56" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E56" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="F56" s="4"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="2:12">
+      <c r="B57" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="B56" t="s">
-        <v>12</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="C57" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E57" s="9" t="s">
         <v>109</v>
       </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>